<commit_message>
12/10 push from lab to home
把terms部分雛型建出來
</commit_message>
<xml_diff>
--- a/piForHo222222企業.xlsx
+++ b/piForHo222222企業.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\桌面\NEW_folder\PI_SP\PI_SP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMS_Workstation\Desktop\excelize_json_practice\excelize_json_practice\PI_SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>NO. 18, DIANZHONG RD.,XIAOGANG DIST., KAOHSIUNG CITY, TAIWAN R.O.C. 81248</t>
   </si>
@@ -247,10 +247,6 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> A) In case of quality discrepancy claim should be filled by the Buyer within 30days after the arrival the goods at port of destination while for quantity discrepancy claim should be</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
     <t>USD</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
@@ -287,7 +283,7 @@
     <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -383,6 +379,12 @@
     </font>
     <font>
       <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -526,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
@@ -570,9 +572,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
@@ -584,9 +583,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
@@ -609,9 +605,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -629,6 +622,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -711,19 +710,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1087,8 +1086,8 @@
   </sheetPr>
   <dimension ref="A1:O994"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="true" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="true"/>
@@ -1110,56 +1109,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="81.75" customHeight="true">
-      <c r="A1" s="35" t="str">
+      <c r="A1" s="34" t="str">
         <f>C7</f>
         <v>PROMETAL INTERNATIONAL CO., LTD</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="true">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1181,23 +1180,19 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="27">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:15" ht="4.5" customHeight="true">
       <c r="A6" s="1"/>
@@ -1211,660 +1206,656 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
     </row>
     <row r="7" spans="1:15" ht="16.5">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="41"/>
+      <c r="I7" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+    </row>
+    <row r="8" spans="1:15" ht="16.5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+    </row>
+    <row r="9" spans="1:15" ht="16.5">
+      <c r="A9" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="41"/>
+      <c r="I9" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+    </row>
+    <row r="10" spans="1:15" ht="16.5">
+      <c r="A10" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.5">
+      <c r="A11" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+    </row>
+    <row r="12" spans="1:15" ht="16.5">
+      <c r="A12" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+    </row>
+    <row r="13" spans="1:15" ht="9.75" customHeight="true">
+      <c r="A13" s="1"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="45"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="29"/>
+    </row>
+    <row r="14" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="29"/>
+    </row>
+    <row r="15" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="29"/>
+    </row>
+    <row r="16" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="29"/>
+    </row>
+    <row r="17" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A17" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="47"/>
+      <c r="F17" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="28" t="s">
-        <v>69</v>
+      <c r="G17" s="49" t="s">
+        <v>15</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="41" t="s">
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="47"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="29"/>
+    </row>
+    <row r="18" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A18" s="50"/>
+      <c r="B18" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="50"/>
+      <c r="F18" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="50"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="29"/>
+    </row>
+    <row r="19" spans="1:15" ht="16.5">
+      <c r="A19" s="18">
+        <v>1</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18">
+        <v>12</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="22">
+        <v>2175</v>
+      </c>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" s="22">
+        <v>26100</v>
+      </c>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+    </row>
+    <row r="20" spans="1:15" ht="16.5">
+      <c r="A20" s="18">
+        <v>2</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18">
+        <v>4</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" s="18">
+        <v>2190</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K20" s="18">
+        <v>8760</v>
+      </c>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+    </row>
+    <row r="21" spans="1:15" ht="16.5">
+      <c r="A21" s="18">
         <v>3</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43" t="s">
-        <v>68</v>
+      <c r="B21" s="18" t="s">
+        <v>49</v>
       </c>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-    </row>
-    <row r="8" spans="1:15" ht="16.5">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-    </row>
-    <row r="9" spans="1:15" ht="16.5">
-      <c r="A9" s="26" t="s">
+      <c r="C21" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
+        <v>5</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" s="18">
+        <v>2390</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="18">
+        <v>11950</v>
+      </c>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+    </row>
+    <row r="22" spans="1:15" ht="16.5">
+      <c r="A22" s="18">
         <v>4</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="43" t="s">
-        <v>74</v>
+      <c r="B22" s="18" t="s">
+        <v>51</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-    </row>
-    <row r="10" spans="1:15" ht="16.5">
-      <c r="A10" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-    </row>
-    <row r="11" spans="1:15" ht="16.5">
-      <c r="A11" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-    </row>
-    <row r="12" spans="1:15" ht="16.5">
-      <c r="A12" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-    </row>
-    <row r="13" spans="1:15" ht="9.75" customHeight="true">
-      <c r="A13" s="28"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="32"/>
-    </row>
-    <row r="14" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A14" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="32"/>
-    </row>
-    <row r="15" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="32"/>
-    </row>
-    <row r="16" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="32"/>
-    </row>
-    <row r="17" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A17" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="48"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="32"/>
-    </row>
-    <row r="18" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A18" s="51"/>
-      <c r="B18" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="51"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="32"/>
-    </row>
-    <row r="19" spans="1:15" ht="16.5">
-      <c r="A19" s="19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>48</v>
+      <c r="D22" s="18" t="s">
+        <v>52</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19">
-        <v>12</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" s="24">
-        <v>2175</v>
-      </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="K19" s="24">
-        <v>26100</v>
-      </c>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-    </row>
-    <row r="20" spans="1:15" ht="16.5">
-      <c r="A20" s="19">
-        <v>2</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
         <v>4</v>
       </c>
-      <c r="G20" s="19" t="s">
-        <v>71</v>
+      <c r="G22" s="18" t="s">
+        <v>70</v>
       </c>
-      <c r="H20" s="19">
-        <v>2190</v>
-      </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="K20" s="19">
-        <v>8760</v>
-      </c>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-    </row>
-    <row r="21" spans="1:15" ht="16.5">
-      <c r="A21" s="19">
-        <v>3</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19">
-        <v>5</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H21" s="19">
-        <v>2390</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="K21" s="19">
-        <v>11950</v>
-      </c>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-    </row>
-    <row r="22" spans="1:15" ht="16.5">
-      <c r="A22" s="19">
-        <v>4</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19">
-        <v>4</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="19">
+      <c r="H22" s="18">
         <v>2300</v>
       </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19" t="s">
-        <v>71</v>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18" t="s">
+        <v>70</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="18">
         <v>9200</v>
       </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
     </row>
     <row r="23" spans="1:15" ht="16.5">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="32"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="29"/>
     </row>
     <row r="24" spans="1:15" ht="18" customHeight="true">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <v>25</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="17">
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="16">
         <v>56010</v>
       </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="32"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" spans="1:15" ht="16.5">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="42"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="41"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="32"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26" spans="1:15" ht="9" customHeight="true">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="32"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="43" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="32"/>
+      <c r="O27" s="29"/>
     </row>
     <row r="28" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="43" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="32"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="32"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="29"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="32"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="32"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="29"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="32"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="24"/>
+      <c r="C31" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="32"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="29"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="32"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="49" t="s">
+      <c r="B32" s="24"/>
+      <c r="C32" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="32"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="29"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="32"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="24"/>
+      <c r="C33" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="32"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="29"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="32"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="32"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="29"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="32"/>
+      <c r="O34" s="29"/>
     </row>
     <row r="35" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="26"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="2" t="s">
         <v>61</v>
       </c>
@@ -1874,18 +1865,18 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="32"/>
+      <c r="J35" s="29"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="32"/>
+      <c r="O35" s="29"/>
     </row>
     <row r="36" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="26"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="2" t="s">
         <v>62</v>
       </c>
@@ -1895,67 +1886,67 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="32"/>
+      <c r="J36" s="29"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="O36" s="32"/>
+      <c r="O36" s="29"/>
     </row>
     <row r="37" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="65" t="s">
-        <v>76</v>
+      <c r="B37" s="41"/>
+      <c r="C37" s="64" t="s">
+        <v>75</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="54"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
-      <c r="O37" s="32"/>
-    </row>
-    <row r="38" spans="1:15" s="15" customFormat="true" ht="13.5" customHeight="true">
-      <c r="A38" s="49"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
+      <c r="O37" s="29"/>
+    </row>
+    <row r="38" spans="1:15" ht="13.5" customHeight="true">
+      <c r="A38" s="48"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
-      <c r="O38" s="32"/>
+      <c r="O38" s="29"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="true">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="32"/>
+      <c r="O39" s="29"/>
     </row>
     <row r="40" spans="1:15" ht="7.5" customHeight="true" thickBot="true">
       <c r="A40" s="9"/>
@@ -1972,336 +1963,334 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="32"/>
+      <c r="O40" s="29"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="55" t="s">
+      <c r="C41" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="56"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="56"/>
-      <c r="J41" s="56"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="55"/>
       <c r="K41" s="10"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="32"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="29"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="58" t="s">
+      <c r="C42" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
       <c r="K42" s="11"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="32"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="29"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="59"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
       <c r="K43" s="11"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="28"/>
-      <c r="O43" s="32"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="29"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="28" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="58" t="s">
+      <c r="C44" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
       <c r="K44" s="11"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="32"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="29"/>
     </row>
     <row r="45" spans="1:15" ht="17.25" thickBot="true">
       <c r="A45" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="60"/>
       <c r="K45" s="13"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="32"/>
-    </row>
-    <row r="46" spans="1:15" s="15" customFormat="true" ht="4.5" customHeight="true">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="32"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="29"/>
+    </row>
+    <row r="46" spans="1:15" ht="4.5" customHeight="true">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="29"/>
     </row>
     <row r="47" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="28"/>
-      <c r="N47" s="28"/>
-      <c r="O47" s="32"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="29"/>
     </row>
     <row r="48">
-      <c r="A48" s="66" t="s">
-        <v>77</v>
+      <c r="A48" s="65" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="66"/>
-    </row>
-    <row r="50" spans="1:15" s="15" customFormat="true" ht="12.75" customHeight="true">
-      <c r="A50" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="64"/>
-      <c r="K50" s="64"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="63"/>
-      <c r="N50" s="63"/>
-      <c r="O50" s="63"/>
+      <c r="A49" s="65"/>
+    </row>
+    <row r="50" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A50" s="65"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="33"/>
+      <c r="N50" s="33"/>
+      <c r="O50" s="33"/>
     </row>
     <row r="51" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A51" s="66"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="62"/>
-      <c r="M51" s="62"/>
-      <c r="N51" s="62"/>
-      <c r="O51" s="62"/>
+      <c r="A51" s="65"/>
+      <c r="B51" s="63"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="63"/>
+      <c r="F51" s="63"/>
+      <c r="G51" s="63"/>
+      <c r="H51" s="63"/>
+      <c r="I51" s="63"/>
+      <c r="J51" s="63"/>
+      <c r="K51" s="63"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="32"/>
+      <c r="N51" s="32"/>
+      <c r="O51" s="32"/>
     </row>
     <row r="52" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A52" s="66"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="28"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="28"/>
-      <c r="N52" s="28"/>
-      <c r="O52" s="32"/>
+      <c r="A52" s="65"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="29"/>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="true">
       <c r="A53" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="28"/>
-      <c r="N53" s="28"/>
-      <c r="O53" s="32"/>
-    </row>
-    <row r="54" spans="1:15" s="20" customFormat="true" ht="15.75" customHeight="true">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="29"/>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" customHeight="true">
       <c r="A54" s="14"/>
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="28"/>
-      <c r="N54" s="28"/>
-      <c r="O54" s="32"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="29"/>
     </row>
     <row r="55" spans="1:15" ht="67.5" customHeight="true">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
-      <c r="J55" s="28"/>
-      <c r="K55" s="28"/>
-      <c r="L55" s="28"/>
-      <c r="M55" s="28"/>
-      <c r="N55" s="28"/>
-      <c r="O55" s="32"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="29"/>
     </row>
     <row r="56" spans="1:15" ht="24.75" customHeight="true">
-      <c r="A56" s="32"/>
-      <c r="B56" s="47" t="s">
+      <c r="A56" s="29"/>
+      <c r="B56" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="47" t="s">
-        <v>74</v>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="46" t="s">
+        <v>73</v>
       </c>
-      <c r="H56" s="48"/>
-      <c r="I56" s="48"/>
-      <c r="J56" s="48"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="28"/>
-      <c r="M56" s="28"/>
-      <c r="N56" s="28"/>
-      <c r="O56" s="32"/>
+      <c r="H56" s="47"/>
+      <c r="I56" s="47"/>
+      <c r="J56" s="47"/>
+      <c r="K56" s="47"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="29"/>
     </row>
     <row r="57" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="28"/>
-      <c r="J57" s="28"/>
-      <c r="K57" s="28"/>
-      <c r="L57" s="28"/>
-      <c r="M57" s="28"/>
-      <c r="N57" s="28"/>
-      <c r="O57" s="32"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="29"/>
     </row>
     <row r="58" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A58" s="28"/>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28"/>
-      <c r="I58" s="28"/>
-      <c r="J58" s="28"/>
-      <c r="K58" s="28"/>
-      <c r="L58" s="28"/>
-      <c r="M58" s="28"/>
-      <c r="N58" s="28"/>
-      <c r="O58" s="32"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="29"/>
     </row>
     <row r="59" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A59" s="28"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
-      <c r="H59" s="28"/>
-      <c r="I59" s="28"/>
-      <c r="J59" s="28"/>
-      <c r="K59" s="28"/>
-      <c r="L59" s="28"/>
-      <c r="M59" s="28"/>
-      <c r="N59" s="28"/>
-      <c r="O59" s="32"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="29"/>
     </row>
     <row r="60" spans="1:15" ht="15.75" customHeight="true">
       <c r="A60" s="1"/>

</xml_diff>

<commit_message>
12/12 home to lab
整體terms都差不多了
剩判斷上下起始位置
</commit_message>
<xml_diff>
--- a/piForHo222222企業.xlsx
+++ b/piForHo222222企業.xlsx
@@ -1,38 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMS_Workstation\Desktop\excelize_json_practice\excelize_json_practice\PI_SP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\桌面\NEW_folder\PI_SP\PI_SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="5625"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>NO. 18, DIANZHONG RD.,XIAOGANG DIST., KAOHSIUNG CITY, TAIWAN R.O.C. 81248</t>
   </si>
@@ -269,10 +256,16 @@
 B) Balance 90% T/T Should Be Remitted Against Copy of B/L</t>
   </si>
   <si>
-    <t xml:space="preserve"> A) In case of quality discrepancy claim should be filled by the Buyer within 30days after the arrival the goods at port of destination while for quantity discrepancy claim should be filled by the Buyer within 15days after the arrival the goods at port of destination. It is understood that the Seller shall not be liable for any discrepancy of goods shipped due to causes for which the Insurance Company, Shipping Company, other transportation organization or post Office are liable.
-B) The Seller shall not be held liable for failure or delay in delivery of the entire lot or a portion of the goods under this sales contract in consequence of any Force Majeure incidents.
-C) The Buyer is requested to sign and return one copy of this Sales Contract immediately after receipt of the same Objection, if any should be raised by the Buyer within five days after the receipt of this Sales Contract in the absence of which it is understood that the Buyer has accepted all the terms and conditions of this Sales Contract.
-D) The price is based on zero export tariff, additional cost shall be borne and paid by the buyer if the export tariff is adjusted by the Chinese government in the future.</t>
+    <t xml:space="preserve"> A) In case of quality discrepancy claim should be filled by the Buyer within 30days after the arrival the goods at port of destination while for quantity discrepancy claim should be filled by the Buyer within 15days after the arrival the goods at port of destination. It is understood that the Seller shall not be liable for any discrepancy of goods shipped due to causes for which the Insurance Company, Shipping Company, other transportation organization or post Office are liable.</t>
+  </si>
+  <si>
+    <t>B) The Seller shall not be held liable for failure or delay in delivery of the entire lot or a portion of the goods under this sales contract in consequence of any Force Majeure incidents.</t>
+  </si>
+  <si>
+    <t>C) The Buyer is requested to sign and return one copy of this Sales Contract immediately after receipt of the same Objection, if any should be raised by the Buyer within five days after the receipt of this Sales Contract in the absence of which it is understood that the Buyer has accepted all the terms and conditions of this Sales Contract.</t>
+  </si>
+  <si>
+    <t>D) The price is based on zero export tariff, additional cost shall be borne and paid by the buyer if the export tariff is adjusted by the Chinese government in the future.</t>
   </si>
 </sst>
 </file>
@@ -283,7 +276,7 @@
     <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -378,25 +371,13 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8.5"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
@@ -528,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
@@ -572,6 +553,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
@@ -583,6 +567,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
@@ -605,6 +592,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -623,11 +613,23 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -689,15 +691,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -710,19 +703,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -1084,10 +1077,10 @@
     <outlinePr summaryBelow="false" summaryRight="false" showOutlineSymbols="false"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:O994"/>
+  <dimension ref="A1:O993"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:K49"/>
+    <sheetView tabSelected="true" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="true"/>
@@ -1109,56 +1102,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="81.75" customHeight="true">
-      <c r="A1" s="34" t="str">
+      <c r="A1" s="41" t="str">
         <f>C7</f>
         <v>PROMETAL INTERNATIONAL CO., LTD</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="true">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1180,19 +1173,23 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="27">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
     </row>
     <row r="6" spans="1:15" ht="4.5" customHeight="true">
       <c r="A6" s="1"/>
@@ -1206,656 +1203,660 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
     </row>
     <row r="7" spans="1:15" ht="16.5">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="40" t="s">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42" t="s">
+      <c r="H7" s="48"/>
+      <c r="I7" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
     </row>
     <row r="8" spans="1:15" ht="16.5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
     </row>
     <row r="9" spans="1:15" ht="16.5">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="42" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="40" t="s">
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="41"/>
-      <c r="I9" s="44" t="s">
+      <c r="H9" s="48"/>
+      <c r="I9" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
     </row>
     <row r="10" spans="1:15" ht="16.5">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="48" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="29"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
     </row>
     <row r="11" spans="1:15" ht="16.5">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="48" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
     </row>
     <row r="12" spans="1:15" ht="16.5">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="24" t="s">
+      <c r="B12" s="32"/>
+      <c r="C12" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
     </row>
     <row r="13" spans="1:15" ht="9.75" customHeight="true">
-      <c r="A13" s="1"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="29"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="32"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="29"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="32"/>
     </row>
     <row r="15" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="29"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="32"/>
     </row>
     <row r="16" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="29"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="32"/>
     </row>
     <row r="17" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="30" t="s">
+      <c r="E17" s="54"/>
+      <c r="F17" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="49" t="s">
+      <c r="G17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="49" t="s">
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="47"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="29"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="32"/>
     </row>
     <row r="18" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A18" s="50"/>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="57"/>
+      <c r="B18" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51" t="s">
+      <c r="C18" s="57"/>
+      <c r="D18" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="50"/>
-      <c r="F18" s="26" t="s">
+      <c r="E18" s="57"/>
+      <c r="F18" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="51" t="s">
+      <c r="G18" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51" t="s">
+      <c r="H18" s="57"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="50"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="29"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="32"/>
     </row>
     <row r="19" spans="1:15" ht="16.5">
-      <c r="A19" s="18">
+      <c r="A19" s="19">
         <v>1</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18">
+      <c r="E19" s="19"/>
+      <c r="F19" s="19">
         <v>12</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="24">
         <v>2175</v>
       </c>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="24">
         <v>26100</v>
       </c>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
     </row>
     <row r="20" spans="1:15" ht="16.5">
-      <c r="A20" s="18">
+      <c r="A20" s="19">
         <v>2</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18">
+      <c r="E20" s="19"/>
+      <c r="F20" s="19">
         <v>4</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="19">
         <v>2190</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18" t="s">
+      <c r="I20" s="19"/>
+      <c r="J20" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="19">
         <v>8760</v>
       </c>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="29"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
     </row>
     <row r="21" spans="1:15" ht="16.5">
-      <c r="A21" s="18">
+      <c r="A21" s="19">
         <v>3</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18">
+      <c r="E21" s="19"/>
+      <c r="F21" s="19">
         <v>5</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="19">
         <v>2390</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18" t="s">
+      <c r="I21" s="19"/>
+      <c r="J21" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="19">
         <v>11950</v>
       </c>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
     </row>
     <row r="22" spans="1:15" ht="16.5">
-      <c r="A22" s="18">
+      <c r="A22" s="19">
         <v>4</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19">
         <v>4</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="19">
         <v>2300</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18" t="s">
+      <c r="I22" s="19"/>
+      <c r="J22" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K22" s="19">
         <v>9200</v>
       </c>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
     </row>
     <row r="23" spans="1:15" ht="16.5">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="29"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="32"/>
     </row>
     <row r="24" spans="1:15" ht="18" customHeight="true">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="23">
         <v>25</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="16">
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="17">
         <v>56010</v>
       </c>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="29"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="32"/>
     </row>
     <row r="25" spans="1:15" ht="16.5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="41"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="48"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="29"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="32"/>
     </row>
     <row r="26" spans="1:15" ht="9" customHeight="true">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="29"/>
+      <c r="O26" s="32"/>
     </row>
     <row r="27" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="42" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="29"/>
+      <c r="O27" s="32"/>
     </row>
     <row r="28" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="42" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="29"/>
+      <c r="O28" s="32"/>
     </row>
     <row r="29" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24" t="s">
+      <c r="B29" s="26"/>
+      <c r="C29" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="29"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="32"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="29"/>
+      <c r="O29" s="32"/>
     </row>
     <row r="30" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24" t="s">
+      <c r="B30" s="26"/>
+      <c r="C30" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="29"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="32"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="29"/>
+      <c r="O30" s="32"/>
     </row>
     <row r="31" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24" t="s">
+      <c r="B31" s="26"/>
+      <c r="C31" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="29"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="32"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="29"/>
+      <c r="O31" s="32"/>
     </row>
     <row r="32" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="48" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="29"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="32"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="29"/>
+      <c r="O32" s="32"/>
     </row>
     <row r="33" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24" t="s">
+      <c r="B33" s="26"/>
+      <c r="C33" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="29"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="32"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="29"/>
+      <c r="O33" s="32"/>
     </row>
     <row r="34" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="29"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="32"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="29"/>
+      <c r="O34" s="32"/>
     </row>
     <row r="35" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="24"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="2" t="s">
         <v>61</v>
       </c>
@@ -1865,18 +1866,18 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="29"/>
+      <c r="J35" s="32"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="29"/>
+      <c r="O35" s="32"/>
     </row>
     <row r="36" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="2" t="s">
         <v>62</v>
       </c>
@@ -1886,67 +1887,67 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="29"/>
+      <c r="J36" s="32"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="O36" s="29"/>
+      <c r="O36" s="32"/>
     </row>
     <row r="37" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="64" t="s">
+      <c r="B37" s="48"/>
+      <c r="C37" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
-      <c r="O37" s="29"/>
-    </row>
-    <row r="38" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A38" s="48"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
+      <c r="O37" s="32"/>
+    </row>
+    <row r="38" spans="1:15" s="15" customFormat="true" ht="13.5" customHeight="true">
+      <c r="A38" s="55"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
-      <c r="O38" s="29"/>
+      <c r="O38" s="32"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="true">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="29"/>
+      <c r="O39" s="32"/>
     </row>
     <row r="40" spans="1:15" ht="7.5" customHeight="true" thickBot="true">
       <c r="A40" s="9"/>
@@ -1963,528 +1964,418 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="29"/>
+      <c r="O40" s="32"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="54" t="s">
+      <c r="C41" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="55"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="66"/>
       <c r="K41" s="10"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="29"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="32"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
       <c r="K42" s="11"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="29"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="32"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="31" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="57" t="s">
+      <c r="C43" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
       <c r="K43" s="11"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="29"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="28"/>
+      <c r="O43" s="32"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
       <c r="K44" s="11"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="29"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="32"/>
     </row>
     <row r="45" spans="1:15" ht="17.25" thickBot="true">
       <c r="A45" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
       <c r="K45" s="13"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="29"/>
-    </row>
-    <row r="46" spans="1:15" ht="4.5" customHeight="true">
-      <c r="A46" s="17"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="29"/>
-    </row>
-    <row r="47" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A47" s="31" t="s">
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="32"/>
+    </row>
+    <row r="46" spans="1:15" s="15" customFormat="true" ht="4.5" customHeight="true">
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="32"/>
+    </row>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A49" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="29"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="65" t="s">
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="28"/>
+      <c r="O49" s="32"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="69" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="65"/>
-    </row>
-    <row r="50" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A50" s="65"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
-      <c r="F50" s="62"/>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
-      <c r="L50" s="33"/>
-      <c r="M50" s="33"/>
-      <c r="N50" s="33"/>
-      <c r="O50" s="33"/>
-    </row>
-    <row r="51" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A51" s="65"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="63"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="63"/>
-      <c r="J51" s="63"/>
-      <c r="K51" s="63"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="O51" s="32"/>
-    </row>
-    <row r="52" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A52" s="65"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="29"/>
-    </row>
-    <row r="53" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A53" s="14" t="s">
+      <c r="B50" s="69"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
+    </row>
+    <row r="51" spans="1:15" s="37" customFormat="true" ht="12.75" customHeight="true">
+      <c r="A51" s="69"/>
+      <c r="B51" s="69"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="69"/>
+      <c r="J51" s="69"/>
+      <c r="K51" s="69"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="36"/>
+    </row>
+    <row r="52" spans="1:15" s="40" customFormat="true" ht="12.75" customHeight="true">
+      <c r="A52" s="69"/>
+      <c r="B52" s="69"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="69"/>
+      <c r="J52" s="69"/>
+      <c r="K52" s="69"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38"/>
+      <c r="O52" s="39"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="69"/>
+      <c r="B53" s="69"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="69"/>
+      <c r="I53" s="69"/>
+      <c r="J53" s="69"/>
+      <c r="K53" s="69"/>
+    </row>
+    <row r="54"/>
+    <row r="55">
+      <c r="A55" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
+      <c r="H55" s="69"/>
+      <c r="I55" s="69"/>
+      <c r="J55" s="69"/>
+      <c r="K55" s="69"/>
+    </row>
+    <row r="56"/>
+    <row r="57">
+      <c r="A57" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="69"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="69"/>
+      <c r="I57" s="69"/>
+      <c r="J57" s="69"/>
+      <c r="K57" s="69"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="69"/>
+      <c r="B58" s="69"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="69"/>
+      <c r="E58" s="69"/>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+      <c r="H58" s="69"/>
+      <c r="I58" s="69"/>
+      <c r="J58" s="69"/>
+      <c r="K58" s="69"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="69"/>
+      <c r="B59" s="69"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="69"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="69"/>
+      <c r="G59" s="69"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="69"/>
+      <c r="J59" s="69"/>
+      <c r="K59" s="69"/>
+    </row>
+    <row r="60"/>
+    <row r="61">
+      <c r="A61" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" s="69"/>
+      <c r="C61" s="69"/>
+      <c r="D61" s="69"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="69"/>
+      <c r="I61" s="69"/>
+      <c r="J61" s="69"/>
+      <c r="K61" s="69"/>
+    </row>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A65" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="29"/>
-    </row>
-    <row r="54" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A54" s="14"/>
-      <c r="B54" s="42" t="s">
-        <v>69</v>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="28"/>
+      <c r="N65" s="28"/>
+      <c r="O65" s="32"/>
+    </row>
+    <row r="66" spans="1:15" s="20" customFormat="true" ht="15.75" customHeight="true">
+      <c r="A66" s="14"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="28"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="28"/>
+      <c r="K66" s="28"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="28"/>
+      <c r="N66" s="28"/>
+      <c r="O66" s="32"/>
+    </row>
+    <row r="67" spans="1:15" ht="67.5" customHeight="true">
+      <c r="A67" s="28"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="28"/>
+      <c r="K67" s="28"/>
+      <c r="L67" s="28"/>
+      <c r="M67" s="28"/>
+      <c r="N67" s="28"/>
+      <c r="O67" s="32"/>
+    </row>
+    <row r="68" spans="1:15" ht="24.75" customHeight="true">
+      <c r="A68" s="32"/>
+      <c r="B68" s="53" t="str">
+        <f>C7</f>
+        <v>PROMETAL INTERNATIONAL CO., LTD</v>
       </c>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="29"/>
-    </row>
-    <row r="55" spans="1:15" ht="67.5" customHeight="true">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="29"/>
-    </row>
-    <row r="56" spans="1:15" ht="24.75" customHeight="true">
-      <c r="A56" s="29"/>
-      <c r="B56" s="46" t="s">
-        <v>69</v>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="53">
+        <f>C9</f>
+        <v>0</v>
       </c>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="H56" s="47"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="47"/>
-      <c r="K56" s="47"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="29"/>
-    </row>
-    <row r="57" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="29"/>
-    </row>
-    <row r="58" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="29"/>
-    </row>
-    <row r="59" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="29"/>
-    </row>
-    <row r="60" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-    </row>
-    <row r="63" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-    </row>
-    <row r="64" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-    </row>
-    <row r="65" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-    </row>
-    <row r="66" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="1:14" ht="15.75" customHeight="true">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-    </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="true">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-    </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="true">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="true">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-    </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="true">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-    </row>
-    <row r="72" spans="1:14" ht="15.75" customHeight="true">
+      <c r="H68" s="54"/>
+      <c r="I68" s="54"/>
+      <c r="J68" s="54"/>
+      <c r="K68" s="54"/>
+      <c r="L68" s="28"/>
+      <c r="M68" s="28"/>
+      <c r="N68" s="28"/>
+      <c r="O68" s="32"/>
+    </row>
+    <row r="69" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+      <c r="K69" s="28"/>
+      <c r="L69" s="28"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="28"/>
+      <c r="O69" s="32"/>
+    </row>
+    <row r="70" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A70" s="28"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="28"/>
+      <c r="H70" s="28"/>
+      <c r="I70" s="28"/>
+      <c r="J70" s="28"/>
+      <c r="K70" s="28"/>
+      <c r="L70" s="28"/>
+      <c r="M70" s="28"/>
+      <c r="N70" s="28"/>
+      <c r="O70" s="32"/>
+    </row>
+    <row r="71" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A71" s="28"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="28"/>
+      <c r="O71" s="32"/>
+    </row>
+    <row r="72" spans="1:15" ht="15.75" customHeight="true">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2500,7 +2391,7 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="true">
+    <row r="73" spans="1:15" ht="15.75" customHeight="true">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2516,7 +2407,7 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
     </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="true">
+    <row r="74" spans="1:15" ht="15.75" customHeight="true">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2532,7 +2423,7 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="1:14" ht="15.75" customHeight="true">
+    <row r="75" spans="1:15" ht="15.75" customHeight="true">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2548,7 +2439,7 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="1:14" ht="15.75" customHeight="true">
+    <row r="76" spans="1:15" ht="15.75" customHeight="true">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2564,7 +2455,7 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75" customHeight="true">
+    <row r="77" spans="1:15" ht="15.75" customHeight="true">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2580,7 +2471,7 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:14" ht="15.75" customHeight="true">
+    <row r="78" spans="1:15" ht="15.75" customHeight="true">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2596,7 +2487,7 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="1:14" ht="15.75" customHeight="true">
+    <row r="79" spans="1:15" ht="15.75" customHeight="true">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -17284,8 +17175,200 @@
       <c r="M996" s="1"/>
       <c r="N996" s="1"/>
     </row>
+    <row r="997" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A997" s="1"/>
+      <c r="B997" s="1"/>
+      <c r="C997" s="1"/>
+      <c r="D997" s="1"/>
+      <c r="E997" s="1"/>
+      <c r="F997" s="1"/>
+      <c r="G997" s="1"/>
+      <c r="H997" s="1"/>
+      <c r="I997" s="1"/>
+      <c r="J997" s="1"/>
+      <c r="K997" s="1"/>
+      <c r="L997" s="1"/>
+      <c r="M997" s="1"/>
+      <c r="N997" s="1"/>
+    </row>
+    <row r="998" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="1"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="1"/>
+      <c r="G998" s="1"/>
+      <c r="H998" s="1"/>
+      <c r="I998" s="1"/>
+      <c r="J998" s="1"/>
+      <c r="K998" s="1"/>
+      <c r="L998" s="1"/>
+      <c r="M998" s="1"/>
+      <c r="N998" s="1"/>
+    </row>
+    <row r="999" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="1"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="1"/>
+      <c r="G999" s="1"/>
+      <c r="H999" s="1"/>
+      <c r="I999" s="1"/>
+      <c r="J999" s="1"/>
+      <c r="K999" s="1"/>
+      <c r="L999" s="1"/>
+      <c r="M999" s="1"/>
+      <c r="N999" s="1"/>
+    </row>
+    <row r="1000" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1000" s="1"/>
+      <c r="B1000" s="1"/>
+      <c r="C1000" s="1"/>
+      <c r="D1000" s="1"/>
+      <c r="E1000" s="1"/>
+      <c r="F1000" s="1"/>
+      <c r="G1000" s="1"/>
+      <c r="H1000" s="1"/>
+      <c r="I1000" s="1"/>
+      <c r="J1000" s="1"/>
+      <c r="K1000" s="1"/>
+      <c r="L1000" s="1"/>
+      <c r="M1000" s="1"/>
+      <c r="N1000" s="1"/>
+    </row>
+    <row r="1001" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+      <c r="G1001" s="1"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="1"/>
+      <c r="J1001" s="1"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="1"/>
+    </row>
+    <row r="1002" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+    </row>
+    <row r="1003" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="1"/>
+      <c r="G1005" s="1"/>
+      <c r="H1005" s="1"/>
+      <c r="I1005" s="1"/>
+      <c r="J1005" s="1"/>
+      <c r="K1005" s="1"/>
+      <c r="L1005" s="1"/>
+      <c r="M1005" s="1"/>
+      <c r="N1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="1"/>
+      <c r="G1006" s="1"/>
+      <c r="H1006" s="1"/>
+      <c r="I1006" s="1"/>
+      <c r="J1006" s="1"/>
+      <c r="K1006" s="1"/>
+      <c r="L1006" s="1"/>
+      <c r="M1006" s="1"/>
+      <c r="N1006" s="1"/>
+    </row>
+    <row r="1007" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="1"/>
+      <c r="G1007" s="1"/>
+      <c r="H1007" s="1"/>
+      <c r="I1007" s="1"/>
+      <c r="J1007" s="1"/>
+      <c r="K1007" s="1"/>
+      <c r="L1007" s="1"/>
+      <c r="M1007" s="1"/>
+      <c r="N1007" s="1"/>
+    </row>
+    <row r="1008" spans="1:14" ht="15.75" customHeight="true">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+      <c r="E1008" s="1"/>
+      <c r="F1008" s="1"/>
+      <c r="G1008" s="1"/>
+      <c r="H1008" s="1"/>
+      <c r="I1008" s="1"/>
+      <c r="J1008" s="1"/>
+      <c r="K1008" s="1"/>
+      <c r="L1008" s="1"/>
+      <c r="M1008" s="1"/>
+      <c r="N1008" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="41">
     <mergeCell ref="C42:J42"/>
     <mergeCell ref="C43:J43"/>
     <mergeCell ref="C44:J44"/>
@@ -17297,8 +17380,8 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="G56:K56"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="G68:K68"/>
     <mergeCell ref="A37:B39"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="I25:J25"/>
@@ -17310,7 +17393,7 @@
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B66:D66"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="G9:H9"/>
@@ -17323,7 +17406,10 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C37:H39"/>
-    <mergeCell ref="A48:K52"/>
+    <mergeCell ref="A50:K53"/>
+    <mergeCell ref="A55:K55"/>
+    <mergeCell ref="A57:K59"/>
+    <mergeCell ref="A61:K61"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
12/12 lab to  home
</commit_message>
<xml_diff>
--- a/piForHo222222企業.xlsx
+++ b/piForHo222222企業.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\桌面\NEW_folder\PI_SP\PI_SP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMS_Workstation\Desktop\excelize_json_practice\excelize_json_practice\PI_SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15675" windowHeight="5625"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -509,7 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
@@ -553,9 +566,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
@@ -567,9 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
@@ -592,9 +599,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -613,23 +617,68 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -647,69 +696,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
@@ -1079,8 +1065,8 @@
   </sheetPr>
   <dimension ref="A1:O993"/>
   <sheetViews>
-    <sheetView tabSelected="true" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="true" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="true"/>
@@ -1102,56 +1088,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="81.75" customHeight="true">
-      <c r="A1" s="41" t="str">
+      <c r="A1" s="53" t="str">
         <f>C7</f>
         <v>PROMETAL INTERNATIONAL CO., LTD</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="true">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1173,23 +1159,19 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="27">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
     </row>
     <row r="6" spans="1:15" ht="4.5" customHeight="true">
       <c r="A6" s="1"/>
@@ -1203,660 +1185,656 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
     </row>
     <row r="7" spans="1:15" ht="16.5">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="47" t="s">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="49" t="s">
+      <c r="H7" s="46"/>
+      <c r="I7" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
     </row>
     <row r="8" spans="1:15" ht="16.5">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="46"/>
       <c r="I8" s="50"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
     </row>
     <row r="9" spans="1:15" ht="16.5">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="49" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="47" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="48"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
     </row>
     <row r="10" spans="1:15" ht="16.5">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="55" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
     </row>
     <row r="11" spans="1:15" ht="16.5">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="55" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
     </row>
     <row r="12" spans="1:15" ht="16.5">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:15" ht="9.75" customHeight="true">
-      <c r="A13" s="28"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="52"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="32"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="29"/>
     </row>
     <row r="14" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="32"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="29"/>
     </row>
     <row r="15" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="32"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="29"/>
     </row>
     <row r="16" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="32"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="29"/>
     </row>
     <row r="17" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="54"/>
-      <c r="F17" s="33" t="s">
+      <c r="E17" s="41"/>
+      <c r="F17" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="56" t="s">
+      <c r="G17" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="56" t="s">
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="54"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="32"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="29"/>
     </row>
     <row r="18" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A18" s="57"/>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58" t="s">
+      <c r="C18" s="43"/>
+      <c r="D18" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="29" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="58" t="s">
+      <c r="G18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="58" t="s">
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="57"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="32"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="29"/>
     </row>
     <row r="19" spans="1:15" ht="16.5">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>1</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19">
+      <c r="E19" s="18"/>
+      <c r="F19" s="18">
         <v>12</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="22">
         <v>2175</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24" t="s">
+      <c r="I19" s="22"/>
+      <c r="J19" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="22">
         <v>26100</v>
       </c>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
     </row>
     <row r="20" spans="1:15" ht="16.5">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <v>2</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18">
         <v>4</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="18">
         <v>2190</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19" t="s">
+      <c r="I20" s="18"/>
+      <c r="J20" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="18">
         <v>8760</v>
       </c>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
     </row>
     <row r="21" spans="1:15" ht="16.5">
-      <c r="A21" s="19">
+      <c r="A21" s="18">
         <v>3</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
         <v>5</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="G21" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="18">
         <v>2390</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19" t="s">
+      <c r="I21" s="18"/>
+      <c r="J21" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="18">
         <v>11950</v>
       </c>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
     </row>
     <row r="22" spans="1:15" ht="16.5">
-      <c r="A22" s="19">
+      <c r="A22" s="18">
         <v>4</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18">
         <v>4</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="G22" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="18">
         <v>2300</v>
       </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19" t="s">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="18">
         <v>9200</v>
       </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
     </row>
     <row r="23" spans="1:15" ht="16.5">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="32"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="29"/>
     </row>
     <row r="24" spans="1:15" ht="18" customHeight="true">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <v>25</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="17">
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="16">
         <v>56010</v>
       </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="32"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="29"/>
     </row>
     <row r="25" spans="1:15" ht="16.5">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="48"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="46"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="32"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="29"/>
     </row>
     <row r="26" spans="1:15" ht="9" customHeight="true">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="32"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="49" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="32"/>
+      <c r="O27" s="29"/>
     </row>
     <row r="28" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="49" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
-      <c r="O28" s="32"/>
+      <c r="O28" s="29"/>
     </row>
     <row r="29" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="32"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="29"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
-      <c r="O29" s="32"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="32"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="29"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="32"/>
+      <c r="O30" s="29"/>
     </row>
     <row r="31" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="24"/>
+      <c r="C31" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="32"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="29"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="32"/>
+      <c r="O31" s="29"/>
     </row>
     <row r="32" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="55" t="s">
+      <c r="B32" s="24"/>
+      <c r="C32" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="32"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="29"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="32"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="24"/>
+      <c r="C33" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="32"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="29"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
-      <c r="O33" s="32"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26" t="s">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="32"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="29"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="32"/>
+      <c r="O34" s="29"/>
     </row>
     <row r="35" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="26"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="2" t="s">
         <v>61</v>
       </c>
@@ -1866,18 +1844,18 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="32"/>
+      <c r="J35" s="29"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="32"/>
+      <c r="O35" s="29"/>
     </row>
     <row r="36" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="26"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="2" t="s">
         <v>62</v>
       </c>
@@ -1887,67 +1865,67 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="32"/>
+      <c r="J36" s="29"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="O36" s="32"/>
+      <c r="O36" s="29"/>
     </row>
     <row r="37" spans="1:15" ht="13.5" customHeight="true">
-      <c r="A37" s="55" t="s">
+      <c r="A37" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="68" t="s">
+      <c r="B37" s="46"/>
+      <c r="C37" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
-      <c r="O37" s="32"/>
-    </row>
-    <row r="38" spans="1:15" s="15" customFormat="true" ht="13.5" customHeight="true">
-      <c r="A38" s="55"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
+      <c r="O37" s="29"/>
+    </row>
+    <row r="38" spans="1:15" ht="13.5" customHeight="true">
+      <c r="A38" s="37"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
-      <c r="O38" s="32"/>
+      <c r="O38" s="29"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="true">
-      <c r="A39" s="48"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="67"/>
-      <c r="H39" s="67"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="32"/>
+      <c r="O39" s="29"/>
     </row>
     <row r="40" spans="1:15" ht="7.5" customHeight="true" thickBot="true">
       <c r="A40" s="9"/>
@@ -1964,416 +1942,446 @@
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
-      <c r="O40" s="32"/>
+      <c r="O40" s="29"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="65" t="s">
+      <c r="C41" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="66"/>
-      <c r="E41" s="66"/>
-      <c r="F41" s="66"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="66"/>
-      <c r="I41" s="66"/>
-      <c r="J41" s="66"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
       <c r="K41" s="10"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="32"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="29"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
       <c r="K42" s="11"/>
-      <c r="L42" s="28"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="32"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="29"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="61" t="s">
+      <c r="C43" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D43" s="62"/>
-      <c r="E43" s="62"/>
-      <c r="F43" s="62"/>
-      <c r="G43" s="62"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="62"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
       <c r="K43" s="11"/>
-      <c r="L43" s="28"/>
-      <c r="M43" s="28"/>
-      <c r="N43" s="28"/>
-      <c r="O43" s="32"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="29"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="28" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="61" t="s">
+      <c r="C44" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
       <c r="K44" s="11"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
-      <c r="O44" s="32"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="29"/>
     </row>
     <row r="45" spans="1:15" ht="17.25" thickBot="true">
       <c r="A45" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="63" t="s">
+      <c r="C45" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
       <c r="K45" s="13"/>
-      <c r="L45" s="28"/>
-      <c r="M45" s="28"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="32"/>
-    </row>
-    <row r="46" spans="1:15" s="15" customFormat="true" ht="4.5" customHeight="true">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="32"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="29"/>
+    </row>
+    <row r="46" spans="1:15" ht="4.5" customHeight="true">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="29"/>
     </row>
     <row r="47"/>
     <row r="48"/>
     <row r="49" spans="1:15" ht="12.75" customHeight="true">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
-      <c r="N49" s="28"/>
-      <c r="O49" s="32"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="29"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="29"/>
     </row>
     <row r="50">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="69"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="69"/>
-      <c r="K50" s="69"/>
-    </row>
-    <row r="51" spans="1:15" s="37" customFormat="true" ht="12.75" customHeight="true">
-      <c r="A51" s="69"/>
-      <c r="B51" s="69"/>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="69"/>
-      <c r="G51" s="69"/>
-      <c r="H51" s="69"/>
-      <c r="I51" s="69"/>
-      <c r="J51" s="69"/>
-      <c r="K51" s="69"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="35"/>
-      <c r="N51" s="35"/>
-      <c r="O51" s="36"/>
-    </row>
-    <row r="52" spans="1:15" s="40" customFormat="true" ht="12.75" customHeight="true">
-      <c r="A52" s="69"/>
-      <c r="B52" s="69"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="69"/>
-      <c r="G52" s="69"/>
-      <c r="H52" s="69"/>
-      <c r="I52" s="69"/>
-      <c r="J52" s="69"/>
-      <c r="K52" s="69"/>
-      <c r="L52" s="38"/>
-      <c r="M52" s="38"/>
-      <c r="N52" s="38"/>
-      <c r="O52" s="39"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="60"/>
+    </row>
+    <row r="51" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A51" s="60"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="60"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="29"/>
+    </row>
+    <row r="52" spans="1:15" ht="12.75" customHeight="true">
+      <c r="A52" s="60"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="60"/>
+      <c r="J52" s="60"/>
+      <c r="K52" s="60"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="29"/>
     </row>
     <row r="53">
-      <c r="A53" s="69"/>
-      <c r="B53" s="69"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="69"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
-      <c r="G53" s="69"/>
-      <c r="H53" s="69"/>
-      <c r="I53" s="69"/>
-      <c r="J53" s="69"/>
-      <c r="K53" s="69"/>
+      <c r="A53" s="60"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="60"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="60"/>
     </row>
     <row r="54"/>
     <row r="55">
-      <c r="A55" s="69" t="s">
+      <c r="A55" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="69"/>
-      <c r="C55" s="69"/>
-      <c r="D55" s="69"/>
-      <c r="E55" s="69"/>
-      <c r="F55" s="69"/>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69"/>
-      <c r="I55" s="69"/>
-      <c r="J55" s="69"/>
-      <c r="K55" s="69"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
+      <c r="F55" s="60"/>
+      <c r="G55" s="60"/>
+      <c r="H55" s="60"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="60"/>
+      <c r="K55" s="60"/>
     </row>
     <row r="56"/>
     <row r="57">
-      <c r="A57" s="69" t="s">
+      <c r="A57" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="69"/>
-      <c r="C57" s="69"/>
-      <c r="D57" s="69"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69"/>
-      <c r="H57" s="69"/>
-      <c r="I57" s="69"/>
-      <c r="J57" s="69"/>
-      <c r="K57" s="69"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="60"/>
+      <c r="I57" s="60"/>
+      <c r="J57" s="60"/>
+      <c r="K57" s="60"/>
     </row>
     <row r="58">
-      <c r="A58" s="69"/>
-      <c r="B58" s="69"/>
-      <c r="C58" s="69"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="69"/>
-      <c r="F58" s="69"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="69"/>
-      <c r="I58" s="69"/>
-      <c r="J58" s="69"/>
-      <c r="K58" s="69"/>
+      <c r="A58" s="60"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="60"/>
+      <c r="F58" s="60"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="60"/>
+      <c r="J58" s="60"/>
+      <c r="K58" s="60"/>
     </row>
     <row r="59">
-      <c r="A59" s="69"/>
-      <c r="B59" s="69"/>
-      <c r="C59" s="69"/>
-      <c r="D59" s="69"/>
-      <c r="E59" s="69"/>
-      <c r="F59" s="69"/>
-      <c r="G59" s="69"/>
-      <c r="H59" s="69"/>
-      <c r="I59" s="69"/>
-      <c r="J59" s="69"/>
-      <c r="K59" s="69"/>
+      <c r="A59" s="60"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="60"/>
+      <c r="F59" s="60"/>
+      <c r="G59" s="60"/>
+      <c r="H59" s="60"/>
+      <c r="I59" s="60"/>
+      <c r="J59" s="60"/>
+      <c r="K59" s="60"/>
     </row>
     <row r="60"/>
     <row r="61">
-      <c r="A61" s="69" t="s">
+      <c r="A61" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="B61" s="69"/>
-      <c r="C61" s="69"/>
-      <c r="D61" s="69"/>
-      <c r="E61" s="69"/>
-      <c r="F61" s="69"/>
-      <c r="G61" s="69"/>
-      <c r="H61" s="69"/>
-      <c r="I61" s="69"/>
-      <c r="J61" s="69"/>
-      <c r="K61" s="69"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="60"/>
     </row>
     <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A65" s="14" t="s">
+    <row r="63" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A63" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B65" s="28"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="28"/>
-      <c r="H65" s="28"/>
-      <c r="I65" s="28"/>
-      <c r="J65" s="28"/>
-      <c r="K65" s="28"/>
-      <c r="L65" s="28"/>
-      <c r="M65" s="28"/>
-      <c r="N65" s="28"/>
-      <c r="O65" s="32"/>
-    </row>
-    <row r="66" spans="1:15" s="20" customFormat="true" ht="15.75" customHeight="true">
-      <c r="A66" s="14"/>
-      <c r="B66" s="49"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="28"/>
-      <c r="J66" s="28"/>
-      <c r="K66" s="28"/>
-      <c r="L66" s="28"/>
-      <c r="M66" s="28"/>
-      <c r="N66" s="28"/>
-      <c r="O66" s="32"/>
-    </row>
-    <row r="67" spans="1:15" ht="67.5" customHeight="true">
-      <c r="A67" s="28"/>
-      <c r="B67" s="28"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="28"/>
-      <c r="K67" s="28"/>
-      <c r="L67" s="28"/>
-      <c r="M67" s="28"/>
-      <c r="N67" s="28"/>
-      <c r="O67" s="32"/>
-    </row>
-    <row r="68" spans="1:15" ht="24.75" customHeight="true">
-      <c r="A68" s="32"/>
-      <c r="B68" s="53" t="str">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="29"/>
+    </row>
+    <row r="64" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A64" s="14"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="29"/>
+    </row>
+    <row r="65" spans="1:15" ht="67.5" customHeight="true">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="29"/>
+    </row>
+    <row r="66" spans="1:15" ht="24.75" customHeight="true">
+      <c r="A66" s="29"/>
+      <c r="B66" s="45" t="str">
         <f>C7</f>
         <v>PROMETAL INTERNATIONAL CO., LTD</v>
       </c>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="53">
+      <c r="C66" s="41"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="45">
         <f>C9</f>
         <v>0</v>
       </c>
-      <c r="H68" s="54"/>
-      <c r="I68" s="54"/>
-      <c r="J68" s="54"/>
-      <c r="K68" s="54"/>
-      <c r="L68" s="28"/>
-      <c r="M68" s="28"/>
-      <c r="N68" s="28"/>
-      <c r="O68" s="32"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="41"/>
+      <c r="K66" s="41"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="29"/>
+    </row>
+    <row r="67" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="29"/>
+    </row>
+    <row r="68" spans="1:15" ht="15.75" customHeight="true">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="29"/>
     </row>
     <row r="69" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="28"/>
-      <c r="N69" s="28"/>
-      <c r="O69" s="32"/>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="29"/>
     </row>
     <row r="70" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A70" s="28"/>
-      <c r="B70" s="28"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="28"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28"/>
-      <c r="K70" s="28"/>
-      <c r="L70" s="28"/>
-      <c r="M70" s="28"/>
-      <c r="N70" s="28"/>
-      <c r="O70" s="32"/>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
     </row>
     <row r="71" spans="1:15" ht="15.75" customHeight="true">
-      <c r="A71" s="28"/>
-      <c r="B71" s="28"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="28"/>
-      <c r="J71" s="28"/>
-      <c r="K71" s="28"/>
-      <c r="L71" s="28"/>
-      <c r="M71" s="28"/>
-      <c r="N71" s="28"/>
-      <c r="O71" s="32"/>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
     </row>
     <row r="72" spans="1:15" ht="15.75" customHeight="true">
       <c r="A72" s="1"/>
@@ -2471,7 +2479,7 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:15" ht="15.75" customHeight="true">
+    <row r="78" spans="1:14" ht="15.75" customHeight="true">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2487,7 +2495,7 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="1:15" ht="15.75" customHeight="true">
+    <row r="79" spans="1:14" ht="15.75" customHeight="true">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -17335,40 +17343,33 @@
       <c r="M1006" s="1"/>
       <c r="N1006" s="1"/>
     </row>
-    <row r="1007" spans="1:14" ht="15.75" customHeight="true">
-      <c r="A1007" s="1"/>
-      <c r="B1007" s="1"/>
-      <c r="C1007" s="1"/>
-      <c r="D1007" s="1"/>
-      <c r="E1007" s="1"/>
-      <c r="F1007" s="1"/>
-      <c r="G1007" s="1"/>
-      <c r="H1007" s="1"/>
-      <c r="I1007" s="1"/>
-      <c r="J1007" s="1"/>
-      <c r="K1007" s="1"/>
-      <c r="L1007" s="1"/>
-      <c r="M1007" s="1"/>
-      <c r="N1007" s="1"/>
-    </row>
-    <row r="1008" spans="1:14" ht="15.75" customHeight="true">
-      <c r="A1008" s="1"/>
-      <c r="B1008" s="1"/>
-      <c r="C1008" s="1"/>
-      <c r="D1008" s="1"/>
-      <c r="E1008" s="1"/>
-      <c r="F1008" s="1"/>
-      <c r="G1008" s="1"/>
-      <c r="H1008" s="1"/>
-      <c r="I1008" s="1"/>
-      <c r="J1008" s="1"/>
-      <c r="K1008" s="1"/>
-      <c r="L1008" s="1"/>
-      <c r="M1008" s="1"/>
-      <c r="N1008" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="G66:K66"/>
+    <mergeCell ref="A37:B39"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C27:J27"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B64:D64"/>
     <mergeCell ref="C42:J42"/>
     <mergeCell ref="C43:J43"/>
     <mergeCell ref="C44:J44"/>
@@ -17380,31 +17381,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="G68:K68"/>
-    <mergeCell ref="A37:B39"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C27:J27"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:K7"/>
     <mergeCell ref="C37:H39"/>
     <mergeCell ref="A50:K53"/>
     <mergeCell ref="A55:K55"/>

</xml_diff>